<commit_message>
updated test data in sheet2
</commit_message>
<xml_diff>
--- a/MACCTests/src/data/testData.xlsx
+++ b/MACCTests/src/data/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="232" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,11 +15,16 @@
     <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>Username</t>
   </si>
@@ -46,6 +51,9 @@
   </si>
   <si>
     <t>hi</t>
+  </si>
+  <si>
+    <t>tahirih</t>
   </si>
   <si>
     <t>Gender</t>
@@ -327,15 +335,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,6 +384,14 @@
       </c>
       <c r="B5" s="0" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>12345</v>
       </c>
     </row>
   </sheetData>
@@ -402,128 +418,128 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>1234</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>234</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>3423</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -548,44 +564,44 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>123</v>
@@ -593,10 +609,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -623,21 +639,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -645,43 +661,43 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -708,73 +724,73 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4744897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>3354364</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,39 +798,39 @@
         <v>342</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3463453</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created Test Plan Template
</commit_message>
<xml_diff>
--- a/MACCTests/src/data/testData.xlsx
+++ b/MACCTests/src/data/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Test Plan" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
   <si>
     <t>Username</t>
   </si>
@@ -213,6 +214,60 @@
   </si>
   <si>
     <t>anywhere</t>
+  </si>
+  <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Pre-Conditions</t>
+  </si>
+  <si>
+    <t>Test Step</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Actual Results</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>1. Check Login Functionality</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>2. Check Sign Up Capabilities</t>
+  </si>
+  <si>
+    <t>Sheet2</t>
+  </si>
+  <si>
+    <t>3. Checking the Posts Functionality</t>
+  </si>
+  <si>
+    <t>Sheet3</t>
+  </si>
+  <si>
+    <t>4. Check User profile Functionalities</t>
+  </si>
+  <si>
+    <t>Sheet4 and sheet5</t>
+  </si>
+  <si>
+    <t>5. Checking for Links</t>
+  </si>
+  <si>
+    <t>5. Checking PeaceTrack Capabilities</t>
   </si>
 </sst>
 </file>
@@ -222,7 +277,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -254,6 +309,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -301,7 +363,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -316,6 +378,18 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -337,14 +411,11 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -418,12 +489,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.0663265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -570,9 +638,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,10 +705,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,13 +789,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0408163265306"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,4 +910,99 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>